<commit_message>
La til støtte for sluttspill. Cleana excel-ark for å lese inn lag.
</commit_message>
<xml_diff>
--- a/PredictionSheets/Rune Brenden - VM 2014 Tippekonkuranse.xlsx
+++ b/PredictionSheets/Rune Brenden - VM 2014 Tippekonkuranse.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\R\Documents\GitHub\VMTipping\PredictionSheets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="0" windowWidth="25365" windowHeight="14265"/>
+    <workbookView xWindow="2100" yWindow="0" windowWidth="25365" windowHeight="14265" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Gruppespilltipp" sheetId="1" r:id="rId1"/>
     <sheet name="Sluttspilltipp" sheetId="2" r:id="rId2"/>
     <sheet name="Kampoppsett" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="132">
   <si>
     <t>Group A</t>
   </si>
@@ -414,9 +419,6 @@
   </si>
   <si>
     <t>Rune Brenden</t>
-  </si>
-  <si>
-    <t>Columbia</t>
   </si>
   <si>
     <t>Italia</t>
@@ -1765,13 +1767,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <tabColor rgb="FFFFFF00"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
@@ -2775,13 +2777,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2821,7 +2823,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>131</v>
+        <v>11</v>
       </c>
       <c r="C5" s="26" t="s">
         <v>21</v>
@@ -2882,7 +2884,7 @@
     </row>
     <row r="12" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="36" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B12" s="37" t="s">
         <v>16</v>
@@ -2945,7 +2947,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <tabColor rgb="FF00B050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>

</xml_diff>